<commit_message>
Update/add mappable files for Xt-EHR
</commit_message>
<xml_diff>
--- a/xtehr/mappable/Condition.xlsx
+++ b/xtehr/mappable/Condition.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,7 +488,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>C.15 - EHDS refined base model for A clinical condition, problem, diagnosis, or other event, situation, issue, or clinical concept that has risen to a level of concern.</t>
+          <t>EHDS refined base model for A clinical condition, problem, diagnosis, or other event, situation, issue, or clinical concept that has risen to a level of concern.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -512,7 +512,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C.15.1 - Identifier</t>
+          <t>Condition identifier</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -535,32 +535,32 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>EHDSCondition.description</t>
+          <t>EHDSCondition.subject</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>EHDSCondition.description</t>
+          <t>EHDSCondition.subject</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C.15.2 - Description</t>
+          <t>Indicates the patient or group who the condition record is associated with.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Condition specification in narrative form</t>
+          <t>Indicates the patient or group who the condition record is associated with.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Narrative</t>
+          <t>EHDSPatient</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0..1</t>
+          <t>1..1</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -568,27 +568,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>EHDSCondition.code</t>
+          <t>EHDSCondition.description</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>EHDSCondition.code</t>
+          <t>EHDSCondition.description</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>C.15.3 - Code</t>
+          <t>Condition specification in narrative form</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Code identifying the condition, problem or diagnosis</t>
+          <t>Condition specification in narrative form</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CodeableConcept</t>
+          <t>string</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -596,36 +596,32 @@
           <t>0..1</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>{'strength': 'preferred', 'description': 'ICD-10*, SNOMED CT, Orphacode if rare disease is diagnosed'}</t>
-        </is>
-      </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EHDSCondition.onsetDate</t>
+          <t>EHDSCondition.code</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>EHDSCondition.onsetDate</t>
+          <t>EHDSCondition.code</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C.15.4 - Onset date</t>
+          <t>Code identifying the condition, problem or diagnosis</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Onset date of a problem/condition</t>
+          <t>Code identifying the condition, problem or diagnosis</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>dateTime</t>
+          <t>CodeableConcept</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -633,27 +629,31 @@
           <t>0..1</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>{'strength': 'preferred', 'description': 'ICD-10*, SNOMED CT, Orphacode if rare disease is diagnosed'}</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>EHDSCondition.endDate</t>
+          <t>EHDSCondition.onsetDate</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>EHDSCondition.endDate</t>
+          <t>EHDSCondition.onsetDate</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>C.15.5 - End date</t>
+          <t>Onset date of a problem/condition</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>The date or estimated date that the condition resolved or went into remission.</t>
+          <t>Onset date of a problem/condition</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -671,32 +671,32 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>EHDSCondition.category</t>
+          <t>EHDSCondition.endDate</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>EHDSCondition.category</t>
+          <t>EHDSCondition.endDate</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C.15.6 - Category</t>
+          <t>The date or estimated date that the condition resolved or went into remission.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Category or categories of the problem.</t>
+          <t>The date or estimated date that the condition resolved or went into remission.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CodeableConcept</t>
+          <t>dateTime</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0..*</t>
+          <t>0..1</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -704,22 +704,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>EHDSCondition.clinicalStatus</t>
+          <t>EHDSCondition.category</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>EHDSCondition.clinicalStatus</t>
+          <t>EHDSCondition.category</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>C.15.7 - Clinical status</t>
+          <t>Category or categories of the problem.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Status of the condition/problem (active, resolved, inactive, ...)</t>
+          <t>Category or categories of the problem.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -729,67 +729,67 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0..1</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>{'strength': 'preferred', 'description': 'HL7 Condtion-clinical'}</t>
-        </is>
-      </c>
+          <t>0..*</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>EHDSCondition.resolutionCircumstances</t>
+          <t>EHDSCondition.clinicalStatus</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>EHDSCondition.resolutionCircumstances</t>
+          <t>EHDSCondition.clinicalStatus</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>C.15.8 - Resolution circumstances</t>
+          <t>Status of the condition/problem (active, resolved, inactive, ...)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Describes the reason for which the status of the problem changed from current to inactive (e.g. surgical procedure, medical treatment, etc.). This field includes "free text" if the resolution circumstances are not already included in other fields such as surgical procedure, medical device, etc., e.g. hepatic cystectomy (this will be the resolution circumstances for the problem "hepatic cyst" and will be included in surgical procedures).</t>
+          <t>Status of the condition/problem (active, resolved, inactive, ...)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>CodeableReference</t>
+          <t>CodeableConcept</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0..*</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr"/>
+          <t>0..1</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>{'strength': 'preferred', 'description': 'HL7 Condition-clinical'}</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>EHDSCondition.severity</t>
+          <t>EHDSCondition.resolutionCircumstances[x]</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>EHDSCondition.severity</t>
+          <t>EHDSCondition.resolutionCircumstances[x]</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>C.15.9 - Severity</t>
+          <t>Describes the reason for which the status of the problem changed from current to inactive (e.g. surgical procedure, medical treatment, etc.).</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>A subjective assessment of the severity of the condition as evaluated by the clinician.</t>
+          <t>This field includes free text if the resolution circumstances are not already included in other fields such as surgical procedure, medical device, etc., e.g. hepatic cystectomy (this will be the resolution circumstances for the problem "hepatic cyst" and will be included in surgical procedures).</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -799,34 +799,30 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0..1</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>{'strength': 'preferred', 'description': 'HL7 Condtion-severity'}</t>
-        </is>
-      </c>
+          <t>0..*</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>EHDSCondition.anatomicLocation</t>
+          <t>EHDSCondition.severity</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>EHDSCondition.anatomicLocation</t>
+          <t>EHDSCondition.severity</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>C.15.10 - Anatomic location</t>
+          <t>A subjective assessment of the severity of the condition as evaluated by the clinician.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>The anatomical location including laterality where this condition manifests itself.</t>
+          <t>A subjective assessment of the severity of the condition as evaluated by the clinician.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -836,34 +832,34 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0..*</t>
+          <t>0..1</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>{'strength': 'preferred', 'description': 'SNOMED CT'}</t>
+          <t>{'strength': 'preferred', 'description': 'HL7 Condition-severity'}</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>EHDSCondition.stage</t>
+          <t>EHDSCondition.anatomicLocation[x]</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>EHDSCondition.stage</t>
+          <t>EHDSCondition.anatomicLocation[x]</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>C.15.11 - Stage</t>
+          <t>The anatomical location including laterality where this condition manifests itself.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Stage/grade usually assessed formally using a specific staging/grading system. Multiple assessment systems could be used.</t>
+          <t>The anatomical location including laterality where this condition manifests itself.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -878,100 +874,108 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>{'strength': 'preferred', 'description': 'e.g. TNM, ICD-O-3, Bi-Rads, Li-Rads, …'}</t>
+          <t>{'strength': 'preferred', 'description': 'SNOMED CT'}</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>EHDSCondition.patient</t>
+          <t>EHDSCondition.stage</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>EHDSCondition.patient</t>
+          <t>EHDSCondition.stage</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>C.15.12 - Subject</t>
+          <t>Stage/grade usually assessed formally using a specific staging/grading system. Multiple assessment systems could be used.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Indicates the patient or group who the condition record is associated with.</t>
+          <t>Stage/grade usually assessed formally using a specific staging/grading system. Multiple assessment systems could be used.</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Reference</t>
+          <t>CodeableConcept</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1..1</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr"/>
+          <t>0..*</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>{'strength': 'preferred', 'description': 'e.g. TNM, ICD-O-3, Bi-Rads, Li-Rads, …'}</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>EHDSCondition.participant</t>
+          <t>EHDSCondition.diagnosisAssertionStatus</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>EHDSCondition.participant</t>
+          <t>EHDSCondition.diagnosisAssertionStatus</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>C.15.13 - Participant</t>
+          <t>Assertion about the certainty associated with a diagnosis. Diagnostic and/or clinical evidence of condition.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Who or what participated in the activities related to the condition and how they were involved.</t>
+          <t>Assertion about the certainty associated with a diagnosis. Diagnostic and/or clinical evidence of condition.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Base</t>
+          <t>CodeableConcept</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0..*</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr"/>
+          <t>0..1</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>{'strength': 'preferred', 'description': 'HL7 Condition-ver-status'}</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>EHDSCondition.participant.function</t>
+          <t>EHDSCondition.asserter</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>EHDSCondition.participant.function</t>
+          <t>EHDSCondition.asserter</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>C.15.13.1 - Function</t>
+          <t>The asserter of the condition</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Type of participant involvement.</t>
+          <t>The asserter of the condition</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>CodeableConcept</t>
+          <t>EHDSHealthProfessional</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -979,114 +983,40 @@
           <t>0..1</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>{'strength': 'preferred', 'description': 'To be specified'}</t>
-        </is>
-      </c>
+      <c r="G16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>EHDSCondition.participant.actor</t>
+          <t>EHDSCondition.assertedDate</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>EHDSCondition.participant.actor</t>
+          <t>EHDSCondition.assertedDate</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>C.15.13.2 - Actor</t>
+          <t>Date and time of the diagnosis assertion</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Identify the Health Professional who may be specifically related to the condition, e.g., as a preferred contact.</t>
+          <t>Date and time of the diagnosis assertion</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Reference</t>
+          <t>dateTime</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>1..1</t>
+          <t>0..1</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>EHDSCondition.externalResourceRelatedWith</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>EHDSCondition.externalResourceRelatedWith</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>C.15.14 - External Resourcerelated with</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Identify the External Resource which may be specifically relatedto the problem, for example a link between a rare disease problemand the corresponding guidelines.</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>uri</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>0..*</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>EHDSCondition.diagnosisAssertionStatus</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>EHDSCondition.diagnosisAssertionStatus</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>C.15.15 - Diagnosis assertion status</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Assertion about the certainty associated with a diagnosis. Diagnostic and/or clinical evidence of condition.</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>CodeableConcept</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>0..1</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>{'strength': 'preferred', 'description': 'HL7 Condition-ver-status'}</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>